<commit_message>
LAA first files added
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Pa.xlsx
+++ b/src/com/data/Test Cases Pa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="60">
   <si>
     <t>TCID</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>BUILD001 :: Yes :: BUILD001 Chief Plan Examiner :: null</t>
+  </si>
+  <si>
+    <t>LaaNew</t>
+  </si>
+  <si>
+    <t>LAA - New</t>
+  </si>
+  <si>
+    <t>Laa :: AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2</t>
   </si>
 </sst>
 </file>
@@ -970,7 +979,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1072,6 +1081,18 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1589,7 +1610,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -1838,7 +1859,9 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="34" t="s">
+        <v>57</v>
+      </c>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -1927,11 +1950,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R12" sqref="R12"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2480,6 +2503,162 @@
       <c r="X14" s="20"/>
       <c r="Y14" s="20"/>
     </row>
+    <row r="19" spans="1:24" s="40" customFormat="1">
+      <c r="A19" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="I19" s="4"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+    </row>
+    <row r="20" spans="1:24" s="36" customFormat="1" ht="25.5">
+      <c r="A20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="N20" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="P20" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q20" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="R20" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="S20" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+    </row>
+    <row r="21" spans="1:24" s="4" customFormat="1" ht="140.25">
+      <c r="A21" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+    </row>
+    <row r="22" spans="1:24" s="42" customFormat="1">
+      <c r="A22" s="24"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="4"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>